<commit_message>
day 1-35, 1-187 confusion fix
Calculation of fisher's exact test using appropriate data.
</commit_message>
<xml_diff>
--- a/data/adverse_events_data.xlsx
+++ b/data/adverse_events_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr.sharepoint.com/sites/ResearchDevelopment-Bioinformatics/Shared Documents/Bioinformatics/Phase1_paper/resubmission/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr.sharepoint.com/sites/ResearchDevelopment-Bioinformatics/Shared Documents/Bioinformatics/Phase1_paper/push_me/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{1DDCDFA6-F6DF-CE42-A3F7-B4D97F62077C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{389C9034-4CEB-6541-9D5D-83DB465FFC43}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="13_ncr:1_{1DDCDFA6-F6DF-CE42-A3F7-B4D97F62077C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AAD58ED-32B1-7348-B359-9F2E3EB1E2A0}"/>
   <bookViews>
-    <workbookView xWindow="28780" yWindow="-1800" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="600" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="adae" sheetId="1" r:id="rId1"/>
@@ -1146,51 +1146,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1224,31 +1180,14 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor theme="0"/>
+          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1263,6 +1202,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1562,16 +1505,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AO36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="AH30" sqref="A20:AH30"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -1715,21 +1660,21 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -1741,61 +1686,58 @@
         <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="L2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>1982390400</v>
+        <v>1965456180</v>
       </c>
       <c r="N2" s="1">
-        <v>44860</v>
+        <v>44664</v>
       </c>
       <c r="O2">
-        <v>1982959200</v>
+        <v>1966024980</v>
       </c>
       <c r="P2" s="1">
-        <v>44866</v>
+        <v>44670</v>
       </c>
       <c r="Q2">
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>133</v>
+        <v>18</v>
       </c>
       <c r="S2" t="s">
-        <v>134</v>
+        <v>19</v>
       </c>
       <c r="T2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="U2" s="1">
-        <v>44893</v>
+        <v>44673</v>
       </c>
       <c r="V2" s="1">
-        <v>44893</v>
-      </c>
-      <c r="X2" t="s">
-        <v>151</v>
+        <v>44673</v>
+      </c>
+      <c r="X2" s="1">
+        <v>44685</v>
       </c>
       <c r="Y2" s="1">
-        <v>44895</v>
-      </c>
-      <c r="Z2">
-        <v>1985420880</v>
+        <v>44685</v>
       </c>
       <c r="AA2">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="AB2">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="AC2" t="s">
         <v>4</v>
@@ -1807,13 +1749,13 @@
         <v>11</v>
       </c>
       <c r="AF2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AI2" t="s">
         <v>11</v>
@@ -1825,27 +1767,27 @@
         <v>14</v>
       </c>
       <c r="AM2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AN2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>23</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
@@ -1857,64 +1799,58 @@
         <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="L3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>1978243560</v>
+        <v>1965456360</v>
       </c>
       <c r="N3" s="1">
-        <v>44812</v>
+        <v>44664</v>
       </c>
       <c r="O3">
-        <v>1978812360</v>
+        <v>1966025160</v>
       </c>
       <c r="P3" s="1">
-        <v>44818</v>
+        <v>44670</v>
       </c>
       <c r="Q3">
         <v>1</v>
       </c>
       <c r="R3" t="s">
-        <v>118</v>
+        <v>24</v>
       </c>
       <c r="S3" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="T3" t="s">
-        <v>44</v>
-      </c>
-      <c r="U3" t="s">
-        <v>119</v>
+        <v>26</v>
+      </c>
+      <c r="U3" s="1">
+        <v>44684</v>
       </c>
       <c r="V3" s="1">
-        <v>44812</v>
-      </c>
-      <c r="W3">
-        <v>1978243560</v>
-      </c>
-      <c r="X3" t="s">
-        <v>120</v>
+        <v>44684</v>
+      </c>
+      <c r="X3" s="1">
+        <v>44698</v>
       </c>
       <c r="Y3" s="1">
-        <v>44815</v>
-      </c>
-      <c r="Z3">
-        <v>1978507020</v>
+        <v>44698</v>
       </c>
       <c r="AA3">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AB3">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="AC3" t="s">
         <v>4</v>
@@ -1938,7 +1874,7 @@
         <v>11</v>
       </c>
       <c r="AJ3" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="AK3" t="s">
         <v>14</v>
@@ -1947,24 +1883,24 @@
         <v>11</v>
       </c>
       <c r="AN3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -1976,64 +1912,61 @@
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="L4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>1978330680</v>
+        <v>1965542940</v>
       </c>
       <c r="N4" s="1">
-        <v>44813</v>
+        <v>44665</v>
       </c>
       <c r="O4">
-        <v>1978899480</v>
+        <v>1966111740</v>
       </c>
       <c r="P4" s="1">
-        <v>44819</v>
+        <v>44671</v>
       </c>
       <c r="Q4">
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="S4" t="s">
-        <v>107</v>
+        <v>30</v>
       </c>
       <c r="T4" t="s">
-        <v>108</v>
+        <v>31</v>
       </c>
       <c r="U4" t="s">
-        <v>109</v>
+        <v>32</v>
       </c>
       <c r="V4" s="1">
-        <v>44816</v>
+        <v>44682</v>
       </c>
       <c r="W4">
-        <v>1978560000</v>
-      </c>
-      <c r="X4" t="s">
-        <v>110</v>
+        <v>1967061600</v>
+      </c>
+      <c r="X4" s="1">
+        <v>44699</v>
       </c>
       <c r="Y4" s="1">
-        <v>44817</v>
-      </c>
-      <c r="Z4">
-        <v>1978697460</v>
+        <v>44699</v>
       </c>
       <c r="AA4">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="AB4">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="AC4" t="s">
         <v>4</v>
@@ -2057,7 +1990,7 @@
         <v>11</v>
       </c>
       <c r="AJ4" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="AK4" t="s">
         <v>14</v>
@@ -2074,16 +2007,16 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
@@ -2095,58 +2028,64 @@
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1968480360</v>
+      </c>
+      <c r="N5" s="1">
+        <v>44699</v>
+      </c>
+      <c r="O5">
+        <v>1969049160</v>
+      </c>
+      <c r="P5" s="1">
+        <v>44705</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>6</v>
+      </c>
+      <c r="S5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T5" t="s">
+        <v>8</v>
+      </c>
+      <c r="U5" t="s">
+        <v>49</v>
+      </c>
+      <c r="V5" s="1">
+        <v>44700</v>
+      </c>
+      <c r="W5">
+        <v>1968604200</v>
+      </c>
+      <c r="X5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>44701</v>
+      </c>
+      <c r="Z5">
+        <v>1968653820</v>
+      </c>
+      <c r="AA5">
+        <v>2</v>
+      </c>
+      <c r="AB5">
         <v>3</v>
-      </c>
-      <c r="K5" t="s">
-        <v>83</v>
-      </c>
-      <c r="L5">
-        <v>3</v>
-      </c>
-      <c r="M5">
-        <v>1978243200</v>
-      </c>
-      <c r="N5" s="1">
-        <v>44812</v>
-      </c>
-      <c r="O5">
-        <v>1978812000</v>
-      </c>
-      <c r="P5" s="1">
-        <v>44818</v>
-      </c>
-      <c r="Q5">
-        <v>2</v>
-      </c>
-      <c r="R5" t="s">
-        <v>102</v>
-      </c>
-      <c r="S5" t="s">
-        <v>103</v>
-      </c>
-      <c r="T5" t="s">
-        <v>79</v>
-      </c>
-      <c r="U5" s="1">
-        <v>44838</v>
-      </c>
-      <c r="V5" s="1">
-        <v>44838</v>
-      </c>
-      <c r="X5" s="1">
-        <v>44853</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>44853</v>
-      </c>
-      <c r="AA5">
-        <v>27</v>
-      </c>
-      <c r="AB5">
-        <v>42</v>
       </c>
       <c r="AC5" t="s">
         <v>4</v>
@@ -2167,10 +2106,10 @@
         <v>12</v>
       </c>
       <c r="AI5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AJ5" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="AK5" t="s">
         <v>14</v>
@@ -2179,24 +2118,24 @@
         <v>11</v>
       </c>
       <c r="AN5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
@@ -2208,64 +2147,64 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="L6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>1978330320</v>
+        <v>1965542940</v>
       </c>
       <c r="N6" s="1">
-        <v>44813</v>
+        <v>44665</v>
       </c>
       <c r="O6">
-        <v>1978899120</v>
+        <v>1966111740</v>
       </c>
       <c r="P6" s="1">
-        <v>44819</v>
+        <v>44671</v>
       </c>
       <c r="Q6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R6" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="S6" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="T6" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="U6" t="s">
-        <v>96</v>
+        <v>32</v>
       </c>
       <c r="V6" s="1">
-        <v>44829</v>
+        <v>44682</v>
       </c>
       <c r="W6">
-        <v>1979719200</v>
+        <v>1967061600</v>
       </c>
       <c r="X6" t="s">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="Y6" s="1">
-        <v>44829</v>
+        <v>44682</v>
       </c>
       <c r="Z6">
-        <v>1979719320</v>
+        <v>1967061660</v>
       </c>
       <c r="AA6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AB6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AC6" t="s">
         <v>4</v>
@@ -2306,10 +2245,10 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2327,25 +2266,25 @@
         <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="L7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>1968480000</v>
+        <v>1968480180</v>
       </c>
       <c r="N7" s="1">
         <v>44699</v>
       </c>
       <c r="O7">
-        <v>1969048800</v>
+        <v>1969048980</v>
       </c>
       <c r="P7" s="1">
         <v>44705</v>
@@ -2354,34 +2293,34 @@
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="S7" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="T7" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="U7" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="V7" s="1">
-        <v>44705</v>
+        <v>44704</v>
       </c>
       <c r="W7">
-        <v>1969017600</v>
+        <v>1968957300</v>
       </c>
       <c r="X7" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="Y7" s="1">
         <v>44705</v>
       </c>
       <c r="Z7">
-        <v>1969017600</v>
+        <v>1969048800</v>
       </c>
       <c r="AA7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB7">
         <v>7</v>
@@ -2405,7 +2344,7 @@
         <v>12</v>
       </c>
       <c r="AI7" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AJ7" t="s">
         <v>41</v>
@@ -2417,24 +2356,24 @@
         <v>11</v>
       </c>
       <c r="AN7" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
         <v>4</v>
@@ -2446,82 +2385,82 @@
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K8" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="L8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M8">
-        <v>1968480000</v>
+        <v>1972886400</v>
       </c>
       <c r="N8" s="1">
-        <v>44699</v>
+        <v>44750</v>
       </c>
       <c r="O8">
-        <v>1969048800</v>
+        <v>1973455200</v>
       </c>
       <c r="P8" s="1">
-        <v>44705</v>
+        <v>44756</v>
       </c>
       <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>59</v>
+      </c>
+      <c r="S8" t="s">
+        <v>60</v>
+      </c>
+      <c r="T8" t="s">
+        <v>61</v>
+      </c>
+      <c r="U8" t="s">
+        <v>62</v>
+      </c>
+      <c r="V8" s="1">
+        <v>44777</v>
+      </c>
+      <c r="W8">
+        <v>1975224780</v>
+      </c>
+      <c r="X8" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>44792</v>
+      </c>
+      <c r="Z8">
+        <v>1976517900</v>
+      </c>
+      <c r="AA8">
+        <v>28</v>
+      </c>
+      <c r="AB8">
+        <v>43</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF8">
         <v>2</v>
       </c>
-      <c r="R8" t="s">
-        <v>42</v>
-      </c>
-      <c r="S8" t="s">
-        <v>43</v>
-      </c>
-      <c r="T8" t="s">
-        <v>44</v>
-      </c>
-      <c r="U8" t="s">
-        <v>45</v>
-      </c>
-      <c r="V8" s="1">
-        <v>44707</v>
-      </c>
-      <c r="W8">
-        <v>1969178400</v>
-      </c>
-      <c r="X8" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y8" s="1">
-        <v>44707</v>
-      </c>
-      <c r="Z8">
-        <v>1969207200</v>
-      </c>
-      <c r="AA8">
-        <v>9</v>
-      </c>
-      <c r="AB8">
-        <v>9</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF8">
-        <v>1</v>
-      </c>
       <c r="AG8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH8" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AI8" t="s">
         <v>11</v>
@@ -2536,7 +2475,7 @@
         <v>11</v>
       </c>
       <c r="AN8" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.2">
@@ -2544,82 +2483,85 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9">
         <v>3</v>
       </c>
-      <c r="F9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
       <c r="K9" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M9">
-        <v>1965542940</v>
+        <v>1978330320</v>
       </c>
       <c r="N9" s="1">
-        <v>44665</v>
+        <v>44813</v>
       </c>
       <c r="O9">
-        <v>1966111740</v>
+        <v>1978899120</v>
       </c>
       <c r="P9" s="1">
-        <v>44671</v>
+        <v>44819</v>
       </c>
       <c r="Q9">
         <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="S9" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="T9" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="U9" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="V9" s="1">
-        <v>44682</v>
+        <v>44819</v>
       </c>
       <c r="W9">
-        <v>1967061600</v>
-      </c>
-      <c r="X9" s="1">
-        <v>44699</v>
+        <v>1978849800</v>
+      </c>
+      <c r="X9" t="s">
+        <v>85</v>
       </c>
       <c r="Y9" s="1">
-        <v>44699</v>
+        <v>44819</v>
+      </c>
+      <c r="Z9">
+        <v>1978876800</v>
       </c>
       <c r="AA9">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="AB9">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="AC9" t="s">
         <v>4</v>
@@ -2640,10 +2582,10 @@
         <v>12</v>
       </c>
       <c r="AI9" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AJ9" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="AK9" t="s">
         <v>14</v>
@@ -2652,7 +2594,7 @@
         <v>11</v>
       </c>
       <c r="AN9" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.2">
@@ -2660,85 +2602,85 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" t="s">
+        <v>83</v>
+      </c>
+      <c r="J10">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
       <c r="K10" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M10">
-        <v>1965542940</v>
+        <v>1978243200</v>
       </c>
       <c r="N10" s="1">
-        <v>44665</v>
+        <v>44812</v>
       </c>
       <c r="O10">
-        <v>1966111740</v>
+        <v>1978812000</v>
       </c>
       <c r="P10" s="1">
-        <v>44671</v>
+        <v>44818</v>
       </c>
       <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10" t="s">
+        <v>42</v>
+      </c>
+      <c r="S10" t="s">
+        <v>43</v>
+      </c>
+      <c r="T10" t="s">
+        <v>44</v>
+      </c>
+      <c r="U10" t="s">
+        <v>100</v>
+      </c>
+      <c r="V10" s="1">
+        <v>44813</v>
+      </c>
+      <c r="W10">
+        <v>1978380900</v>
+      </c>
+      <c r="X10" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>44814</v>
+      </c>
+      <c r="Z10">
+        <v>1978407180</v>
+      </c>
+      <c r="AA10">
         <v>2</v>
       </c>
-      <c r="R10" t="s">
-        <v>33</v>
-      </c>
-      <c r="S10" t="s">
-        <v>34</v>
-      </c>
-      <c r="T10" t="s">
-        <v>31</v>
-      </c>
-      <c r="U10" t="s">
-        <v>32</v>
-      </c>
-      <c r="V10" s="1">
-        <v>44682</v>
-      </c>
-      <c r="W10">
-        <v>1967061600</v>
-      </c>
-      <c r="X10" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y10" s="1">
-        <v>44682</v>
-      </c>
-      <c r="Z10">
-        <v>1967061660</v>
-      </c>
-      <c r="AA10">
-        <v>18</v>
-      </c>
       <c r="AB10">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AC10" t="s">
         <v>4</v>
@@ -2759,10 +2701,10 @@
         <v>12</v>
       </c>
       <c r="AI10" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AJ10" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="AK10" t="s">
         <v>14</v>
@@ -2771,87 +2713,93 @@
         <v>11</v>
       </c>
       <c r="AN10" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J11">
         <v>3</v>
       </c>
-      <c r="F11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
       <c r="K11" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M11">
-        <v>1965456360</v>
+        <v>1978330680</v>
       </c>
       <c r="N11" s="1">
-        <v>44664</v>
+        <v>44813</v>
       </c>
       <c r="O11">
-        <v>1966025160</v>
+        <v>1978899480</v>
       </c>
       <c r="P11" s="1">
-        <v>44670</v>
+        <v>44819</v>
       </c>
       <c r="Q11">
         <v>1</v>
       </c>
       <c r="R11" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="S11" t="s">
-        <v>25</v>
+        <v>107</v>
       </c>
       <c r="T11" t="s">
-        <v>26</v>
-      </c>
-      <c r="U11" s="1">
-        <v>44684</v>
+        <v>108</v>
+      </c>
+      <c r="U11" t="s">
+        <v>109</v>
       </c>
       <c r="V11" s="1">
-        <v>44684</v>
-      </c>
-      <c r="X11" s="1">
-        <v>44698</v>
+        <v>44816</v>
+      </c>
+      <c r="W11">
+        <v>1978560000</v>
+      </c>
+      <c r="X11" t="s">
+        <v>110</v>
       </c>
       <c r="Y11" s="1">
-        <v>44698</v>
+        <v>44817</v>
+      </c>
+      <c r="Z11">
+        <v>1978697460</v>
       </c>
       <c r="AA11">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="AB11">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="AC11" t="s">
         <v>4</v>
@@ -2875,7 +2823,7 @@
         <v>11</v>
       </c>
       <c r="AJ11" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="AK11" t="s">
         <v>14</v>
@@ -2887,90 +2835,90 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>81</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12">
         <v>3</v>
       </c>
-      <c r="F12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12">
-        <v>4</v>
-      </c>
       <c r="K12" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="L12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M12">
-        <v>1965456000</v>
+        <v>1978330320</v>
       </c>
       <c r="N12" s="1">
-        <v>44664</v>
+        <v>44813</v>
       </c>
       <c r="O12">
-        <v>1966024800</v>
+        <v>1978899120</v>
       </c>
       <c r="P12" s="1">
-        <v>44670</v>
+        <v>44819</v>
       </c>
       <c r="Q12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R12" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="S12" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="T12" t="s">
         <v>8</v>
       </c>
       <c r="U12" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="V12" s="1">
-        <v>44677</v>
+        <v>44829</v>
       </c>
       <c r="W12">
-        <v>1966574400</v>
+        <v>1979719200</v>
       </c>
       <c r="X12" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="Y12" s="1">
-        <v>44677</v>
+        <v>44829</v>
       </c>
       <c r="Z12">
-        <v>1966574460</v>
+        <v>1979719320</v>
       </c>
       <c r="AA12">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="AB12">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="AC12" t="s">
         <v>4</v>
@@ -3003,18 +2951,18 @@
         <v>11</v>
       </c>
       <c r="AN12" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -3032,64 +2980,61 @@
         <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="J13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K13" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="L13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M13">
-        <v>1981180980</v>
+        <v>1982390400</v>
       </c>
       <c r="N13" s="1">
-        <v>44846</v>
+        <v>44860</v>
       </c>
       <c r="O13">
-        <v>1981749780</v>
+        <v>1982959200</v>
       </c>
       <c r="P13" s="1">
-        <v>44852</v>
+        <v>44866</v>
       </c>
       <c r="Q13">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="S13" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="T13" t="s">
-        <v>61</v>
-      </c>
-      <c r="U13" t="s">
-        <v>144</v>
+        <v>8</v>
+      </c>
+      <c r="U13" s="1">
+        <v>44893</v>
       </c>
       <c r="V13" s="1">
-        <v>44847</v>
-      </c>
-      <c r="W13">
-        <v>1981266180</v>
+        <v>44893</v>
       </c>
       <c r="X13" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="Y13" s="1">
-        <v>44855</v>
+        <v>44895</v>
       </c>
       <c r="Z13">
-        <v>1981959300</v>
+        <v>1985420880</v>
       </c>
       <c r="AA13">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="AB13">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="AC13" t="s">
         <v>4</v>
@@ -3110,10 +3055,10 @@
         <v>12</v>
       </c>
       <c r="AI13" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AJ13" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="AK13" t="s">
         <v>14</v>
@@ -3125,15 +3070,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -3151,64 +3096,64 @@
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="J14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K14" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="L14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M14">
-        <v>1979971380</v>
+        <v>1978330320</v>
       </c>
       <c r="N14" s="1">
-        <v>44832</v>
+        <v>44813</v>
       </c>
       <c r="O14">
-        <v>1980540180</v>
+        <v>1978899120</v>
       </c>
       <c r="P14" s="1">
-        <v>44838</v>
+        <v>44819</v>
       </c>
       <c r="Q14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R14" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="S14" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="T14" t="s">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="U14" t="s">
-        <v>138</v>
+        <v>89</v>
       </c>
       <c r="V14" s="1">
-        <v>44838</v>
+        <v>44829</v>
       </c>
       <c r="W14">
-        <v>1980514380</v>
+        <v>1979701200</v>
       </c>
       <c r="X14" t="s">
-        <v>139</v>
+        <v>90</v>
       </c>
       <c r="Y14" s="1">
-        <v>44839</v>
+        <v>44844</v>
       </c>
       <c r="Z14">
-        <v>1980567120</v>
+        <v>1981004520</v>
       </c>
       <c r="AA14">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="AB14">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="AC14" t="s">
         <v>4</v>
@@ -3220,19 +3165,19 @@
         <v>11</v>
       </c>
       <c r="AF14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH14" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AI14" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AJ14" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="AK14" t="s">
         <v>14</v>
@@ -3241,18 +3186,18 @@
         <v>11</v>
       </c>
       <c r="AN14" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -3282,13 +3227,13 @@
         <v>3</v>
       </c>
       <c r="M15">
-        <v>1978330680</v>
+        <v>1978330320</v>
       </c>
       <c r="N15" s="1">
         <v>44813</v>
       </c>
       <c r="O15">
-        <v>1978899480</v>
+        <v>1978899120</v>
       </c>
       <c r="P15" s="1">
         <v>44819</v>
@@ -3297,37 +3242,37 @@
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="S15" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="T15" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="U15" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="V15" s="1">
-        <v>44816</v>
+        <v>44829</v>
       </c>
       <c r="W15">
-        <v>1978599600</v>
+        <v>1979701200</v>
       </c>
       <c r="X15" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="Y15" s="1">
-        <v>44816</v>
+        <v>44829</v>
       </c>
       <c r="Z15">
-        <v>1978621200</v>
+        <v>1979760600</v>
       </c>
       <c r="AA15">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="AB15">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="AC15" t="s">
         <v>4</v>
@@ -3339,19 +3284,19 @@
         <v>11</v>
       </c>
       <c r="AF15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH15" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AI15" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AJ15" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="AK15" t="s">
         <v>14</v>
@@ -3360,10 +3305,10 @@
         <v>11</v>
       </c>
       <c r="AN15" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -3413,40 +3358,34 @@
         <v>44818</v>
       </c>
       <c r="Q16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R16" t="s">
+        <v>102</v>
+      </c>
+      <c r="S16" t="s">
+        <v>103</v>
+      </c>
+      <c r="T16" t="s">
+        <v>79</v>
+      </c>
+      <c r="U16" s="1">
+        <v>44838</v>
+      </c>
+      <c r="V16" s="1">
+        <v>44838</v>
+      </c>
+      <c r="X16" s="1">
+        <v>44853</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>44853</v>
+      </c>
+      <c r="AA16">
+        <v>27</v>
+      </c>
+      <c r="AB16">
         <v>42</v>
-      </c>
-      <c r="S16" t="s">
-        <v>43</v>
-      </c>
-      <c r="T16" t="s">
-        <v>44</v>
-      </c>
-      <c r="U16" t="s">
-        <v>100</v>
-      </c>
-      <c r="V16" s="1">
-        <v>44813</v>
-      </c>
-      <c r="W16">
-        <v>1978380900</v>
-      </c>
-      <c r="X16" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y16" s="1">
-        <v>44814</v>
-      </c>
-      <c r="Z16">
-        <v>1978407180</v>
-      </c>
-      <c r="AA16">
-        <v>2</v>
-      </c>
-      <c r="AB16">
-        <v>3</v>
       </c>
       <c r="AC16" t="s">
         <v>4</v>
@@ -3467,10 +3406,10 @@
         <v>12</v>
       </c>
       <c r="AI16" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AJ16" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="AK16" t="s">
         <v>14</v>
@@ -3479,7 +3418,7 @@
         <v>11</v>
       </c>
       <c r="AN16" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.2">
@@ -3487,10 +3426,10 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -3520,19 +3459,19 @@
         <v>3</v>
       </c>
       <c r="M17">
-        <v>1978330320</v>
+        <v>1978330680</v>
       </c>
       <c r="N17" s="1">
         <v>44813</v>
       </c>
       <c r="O17">
-        <v>1978899120</v>
+        <v>1978899480</v>
       </c>
       <c r="P17" s="1">
         <v>44819</v>
       </c>
       <c r="Q17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R17" t="s">
         <v>42</v>
@@ -3544,28 +3483,28 @@
         <v>44</v>
       </c>
       <c r="U17" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="V17" s="1">
-        <v>44819</v>
+        <v>44816</v>
       </c>
       <c r="W17">
-        <v>1978849800</v>
+        <v>1978599600</v>
       </c>
       <c r="X17" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="Y17" s="1">
-        <v>44819</v>
+        <v>44816</v>
       </c>
       <c r="Z17">
-        <v>1978876800</v>
+        <v>1978621200</v>
       </c>
       <c r="AA17">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AB17">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AC17" t="s">
         <v>4</v>
@@ -3601,90 +3540,87 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" t="s">
+        <v>83</v>
+      </c>
+      <c r="J18">
         <v>3</v>
       </c>
-      <c r="F18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" t="s">
-        <v>4</v>
-      </c>
-      <c r="I18" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
       <c r="K18" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M18">
-        <v>1968480180</v>
+        <v>1978330680</v>
       </c>
       <c r="N18" s="1">
-        <v>44699</v>
+        <v>44813</v>
       </c>
       <c r="O18">
-        <v>1969048980</v>
+        <v>1978899480</v>
       </c>
       <c r="P18" s="1">
-        <v>44705</v>
+        <v>44819</v>
       </c>
       <c r="Q18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R18" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="S18" t="s">
-        <v>43</v>
+        <v>114</v>
       </c>
       <c r="T18" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="U18" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="V18" s="1">
-        <v>44704</v>
+        <v>44834</v>
       </c>
       <c r="W18">
-        <v>1968957300</v>
-      </c>
-      <c r="X18" t="s">
-        <v>54</v>
+        <v>1980154800</v>
+      </c>
+      <c r="X18" s="1">
+        <v>44879</v>
       </c>
       <c r="Y18" s="1">
-        <v>44705</v>
-      </c>
-      <c r="Z18">
-        <v>1969048800</v>
+        <v>44879</v>
       </c>
       <c r="AA18">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="AB18">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="AC18" t="s">
         <v>4</v>
@@ -3696,19 +3632,19 @@
         <v>11</v>
       </c>
       <c r="AF18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH18" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AI18" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AJ18" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="AK18" t="s">
         <v>14</v>
@@ -3717,117 +3653,114 @@
         <v>11</v>
       </c>
       <c r="AN18" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>146</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>147</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19">
         <v>3</v>
       </c>
-      <c r="F19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" t="s">
-        <v>4</v>
-      </c>
-      <c r="H19" t="s">
-        <v>4</v>
-      </c>
-      <c r="I19" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
       <c r="K19" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M19">
-        <v>1968480360</v>
+        <v>1982390400</v>
       </c>
       <c r="N19" s="1">
-        <v>44699</v>
+        <v>44860</v>
       </c>
       <c r="O19">
-        <v>1969049160</v>
+        <v>1982959200</v>
       </c>
       <c r="P19" s="1">
-        <v>44705</v>
+        <v>44866</v>
       </c>
       <c r="Q19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R19" t="s">
-        <v>6</v>
+        <v>148</v>
       </c>
       <c r="S19" t="s">
-        <v>7</v>
+        <v>149</v>
       </c>
       <c r="T19" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="U19" t="s">
-        <v>49</v>
+        <v>150</v>
       </c>
       <c r="V19" s="1">
-        <v>44700</v>
+        <v>44870</v>
       </c>
       <c r="W19">
-        <v>1968604200</v>
-      </c>
-      <c r="X19" t="s">
-        <v>50</v>
+        <v>1983267000</v>
+      </c>
+      <c r="X19" s="1">
+        <v>44883</v>
       </c>
       <c r="Y19" s="1">
-        <v>44701</v>
-      </c>
-      <c r="Z19">
-        <v>1968653820</v>
+        <v>44883</v>
       </c>
       <c r="AA19">
+        <v>11</v>
+      </c>
+      <c r="AB19">
+        <v>24</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF19">
         <v>2</v>
       </c>
-      <c r="AB19">
-        <v>3</v>
-      </c>
-      <c r="AC19" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF19">
-        <v>1</v>
-      </c>
       <c r="AG19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH19" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="AI19" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AJ19" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="AK19" t="s">
         <v>14</v>
@@ -3836,24 +3769,24 @@
         <v>11</v>
       </c>
       <c r="AN19" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>146</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>147</v>
+        <v>37</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="F20" t="s">
         <v>4</v>
@@ -3865,61 +3798,64 @@
         <v>4</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="J20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K20" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="L20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M20">
-        <v>1982390400</v>
+        <v>1968480000</v>
       </c>
       <c r="N20" s="1">
-        <v>44860</v>
+        <v>44699</v>
       </c>
       <c r="O20">
-        <v>1982959200</v>
+        <v>1969048800</v>
       </c>
       <c r="P20" s="1">
-        <v>44866</v>
+        <v>44705</v>
       </c>
       <c r="Q20">
         <v>2</v>
       </c>
       <c r="R20" t="s">
-        <v>148</v>
+        <v>42</v>
       </c>
       <c r="S20" t="s">
-        <v>149</v>
+        <v>43</v>
       </c>
       <c r="T20" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="U20" t="s">
-        <v>150</v>
+        <v>45</v>
       </c>
       <c r="V20" s="1">
-        <v>44870</v>
+        <v>44707</v>
       </c>
       <c r="W20">
-        <v>1983267000</v>
-      </c>
-      <c r="X20" s="1">
-        <v>44883</v>
+        <v>1969178400</v>
+      </c>
+      <c r="X20" t="s">
+        <v>46</v>
       </c>
       <c r="Y20" s="1">
-        <v>44883</v>
+        <v>44707</v>
+      </c>
+      <c r="Z20">
+        <v>1969207200</v>
       </c>
       <c r="AA20">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AB20">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="AC20" t="s">
         <v>4</v>
@@ -3931,13 +3867,13 @@
         <v>11</v>
       </c>
       <c r="AF20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH20" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AI20" t="s">
         <v>11</v>
@@ -3952,24 +3888,24 @@
         <v>11</v>
       </c>
       <c r="AN20" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F21" t="s">
         <v>4</v>
@@ -3993,70 +3929,67 @@
         <v>4</v>
       </c>
       <c r="M21">
-        <v>1978935300</v>
+        <v>1972886580</v>
       </c>
       <c r="N21" s="1">
-        <v>44820</v>
+        <v>44750</v>
       </c>
       <c r="O21">
-        <v>1979504100</v>
+        <v>1973455380</v>
       </c>
       <c r="P21" s="1">
-        <v>44826</v>
+        <v>44756</v>
       </c>
       <c r="Q21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R21" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="S21" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="T21" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="U21" t="s">
-        <v>128</v>
+        <v>68</v>
       </c>
       <c r="V21" s="1">
-        <v>44850</v>
+        <v>44764</v>
       </c>
       <c r="W21">
-        <v>1981540800</v>
-      </c>
-      <c r="X21" t="s">
-        <v>129</v>
+        <v>1974072600</v>
+      </c>
+      <c r="X21" s="1">
+        <v>44796</v>
       </c>
       <c r="Y21" s="1">
-        <v>44852</v>
-      </c>
-      <c r="Z21">
-        <v>1981699200</v>
+        <v>44796</v>
       </c>
       <c r="AA21">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="AB21">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="AC21" t="s">
         <v>4</v>
       </c>
       <c r="AD21" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AE21" t="s">
         <v>11</v>
       </c>
       <c r="AF21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH21" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="AI21" t="s">
         <v>11</v>
@@ -4067,28 +4000,34 @@
       <c r="AK21" t="s">
         <v>14</v>
       </c>
+      <c r="AL21" t="s">
+        <v>11</v>
+      </c>
       <c r="AM21" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AN21" t="s">
         <v>11</v>
       </c>
+      <c r="AO21" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F22" t="s">
         <v>4</v>
@@ -4112,67 +4051,67 @@
         <v>4</v>
       </c>
       <c r="M22">
-        <v>1978935300</v>
+        <v>1972886580</v>
       </c>
       <c r="N22" s="1">
-        <v>44820</v>
+        <v>44750</v>
       </c>
       <c r="O22">
-        <v>1979504100</v>
+        <v>1973455380</v>
       </c>
       <c r="P22" s="1">
+        <v>44756</v>
+      </c>
+      <c r="Q22">
+        <v>4</v>
+      </c>
+      <c r="R22" t="s">
+        <v>75</v>
+      </c>
+      <c r="S22" t="s">
+        <v>76</v>
+      </c>
+      <c r="T22" t="s">
+        <v>31</v>
+      </c>
+      <c r="U22" t="s">
+        <v>68</v>
+      </c>
+      <c r="V22" s="1">
+        <v>44764</v>
+      </c>
+      <c r="W22">
+        <v>1974072600</v>
+      </c>
+      <c r="X22" s="1">
         <v>44826</v>
       </c>
-      <c r="Q22">
-        <v>2</v>
-      </c>
-      <c r="R22" t="s">
-        <v>102</v>
-      </c>
-      <c r="S22" t="s">
-        <v>103</v>
-      </c>
-      <c r="T22" t="s">
-        <v>79</v>
-      </c>
-      <c r="U22" t="s">
-        <v>130</v>
-      </c>
-      <c r="V22" s="1">
-        <v>44851</v>
-      </c>
-      <c r="W22">
-        <v>1981612800</v>
-      </c>
-      <c r="X22" s="1">
-        <v>44858</v>
-      </c>
       <c r="Y22" s="1">
-        <v>44858</v>
+        <v>44826</v>
       </c>
       <c r="AA22">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="AB22">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="AC22" t="s">
         <v>4</v>
       </c>
       <c r="AD22" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AE22" t="s">
         <v>11</v>
       </c>
       <c r="AF22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH22" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="AI22" t="s">
         <v>11</v>
@@ -4183,28 +4122,34 @@
       <c r="AK22" t="s">
         <v>14</v>
       </c>
+      <c r="AL22" t="s">
+        <v>11</v>
+      </c>
       <c r="AM22" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AN22" t="s">
         <v>11</v>
       </c>
+      <c r="AO22" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>117</v>
+        <v>65</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s">
         <v>4</v>
@@ -4228,70 +4173,70 @@
         <v>4</v>
       </c>
       <c r="M23">
-        <v>1978243560</v>
+        <v>1972886580</v>
       </c>
       <c r="N23" s="1">
-        <v>44812</v>
+        <v>44750</v>
       </c>
       <c r="O23">
-        <v>1978812360</v>
+        <v>1973455380</v>
       </c>
       <c r="P23" s="1">
-        <v>44818</v>
+        <v>44756</v>
       </c>
       <c r="Q23">
         <v>3</v>
       </c>
       <c r="R23" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="S23" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="T23" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="U23" t="s">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="V23" s="1">
-        <v>44831</v>
+        <v>44764</v>
       </c>
       <c r="W23">
-        <v>1979916300</v>
+        <v>1974072600</v>
       </c>
       <c r="X23" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="Y23" s="1">
-        <v>44831</v>
+        <v>44764</v>
       </c>
       <c r="Z23">
-        <v>1979920800</v>
+        <v>1974072660</v>
       </c>
       <c r="AA23">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="AB23">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="AC23" t="s">
         <v>4</v>
       </c>
       <c r="AD23" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AE23" t="s">
         <v>11</v>
       </c>
       <c r="AF23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AG23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH23" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="AI23" t="s">
         <v>11</v>
@@ -4302,28 +4247,34 @@
       <c r="AK23" t="s">
         <v>14</v>
       </c>
+      <c r="AL23" t="s">
+        <v>11</v>
+      </c>
       <c r="AM23" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AN23" t="s">
         <v>11</v>
       </c>
+      <c r="AO23" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>117</v>
+        <v>2</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="F24" t="s">
         <v>4</v>
@@ -4347,52 +4298,52 @@
         <v>4</v>
       </c>
       <c r="M24">
-        <v>1978243560</v>
+        <v>1965456000</v>
       </c>
       <c r="N24" s="1">
-        <v>44812</v>
+        <v>44664</v>
       </c>
       <c r="O24">
-        <v>1978812360</v>
+        <v>1966024800</v>
       </c>
       <c r="P24" s="1">
-        <v>44818</v>
+        <v>44670</v>
       </c>
       <c r="Q24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R24" t="s">
-        <v>121</v>
+        <v>6</v>
       </c>
       <c r="S24" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="T24" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="U24" t="s">
-        <v>122</v>
+        <v>9</v>
       </c>
       <c r="V24" s="1">
-        <v>44819</v>
+        <v>44677</v>
       </c>
       <c r="W24">
-        <v>1978866000</v>
+        <v>1966574400</v>
       </c>
       <c r="X24" t="s">
-        <v>123</v>
+        <v>10</v>
       </c>
       <c r="Y24" s="1">
-        <v>44819</v>
+        <v>44677</v>
       </c>
       <c r="Z24">
-        <v>1978891200</v>
+        <v>1966574460</v>
       </c>
       <c r="AA24">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="AB24">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="AC24" t="s">
         <v>4</v>
@@ -4404,13 +4355,13 @@
         <v>11</v>
       </c>
       <c r="AF24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH24" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AI24" t="s">
         <v>11</v>
@@ -4428,21 +4379,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
+        <v>37</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="F25" t="s">
         <v>4</v>
@@ -4454,61 +4405,64 @@
         <v>4</v>
       </c>
       <c r="I25" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="J25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K25" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="L25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M25">
-        <v>1978330680</v>
+        <v>1968480000</v>
       </c>
       <c r="N25" s="1">
-        <v>44813</v>
+        <v>44699</v>
       </c>
       <c r="O25">
-        <v>1978899480</v>
+        <v>1969048800</v>
       </c>
       <c r="P25" s="1">
-        <v>44819</v>
+        <v>44705</v>
       </c>
       <c r="Q25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R25" t="s">
-        <v>113</v>
+        <v>38</v>
       </c>
       <c r="S25" t="s">
-        <v>114</v>
+        <v>39</v>
       </c>
       <c r="T25" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="U25" t="s">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="V25" s="1">
-        <v>44834</v>
+        <v>44705</v>
       </c>
       <c r="W25">
-        <v>1980154800</v>
-      </c>
-      <c r="X25" s="1">
-        <v>44879</v>
+        <v>1969017600</v>
+      </c>
+      <c r="X25" t="s">
+        <v>40</v>
       </c>
       <c r="Y25" s="1">
-        <v>44879</v>
+        <v>44705</v>
+      </c>
+      <c r="Z25">
+        <v>1969017600</v>
       </c>
       <c r="AA25">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="AB25">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="AC25" t="s">
         <v>4</v>
@@ -4520,19 +4474,19 @@
         <v>11</v>
       </c>
       <c r="AF25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH25" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AI25" t="s">
         <v>11</v>
       </c>
       <c r="AJ25" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="AK25" t="s">
         <v>14</v>
@@ -4544,21 +4498,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F26" t="s">
         <v>4</v>
@@ -4570,82 +4524,79 @@
         <v>4</v>
       </c>
       <c r="I26" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="J26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K26" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="L26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M26">
-        <v>1978330320</v>
+        <v>1972886580</v>
       </c>
       <c r="N26" s="1">
-        <v>44813</v>
+        <v>44750</v>
       </c>
       <c r="O26">
-        <v>1978899120</v>
+        <v>1973455380</v>
       </c>
       <c r="P26" s="1">
-        <v>44819</v>
+        <v>44756</v>
       </c>
       <c r="Q26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R26" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="S26" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="T26" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="U26" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="V26" s="1">
-        <v>44829</v>
+        <v>44764</v>
       </c>
       <c r="W26">
-        <v>1979701200</v>
-      </c>
-      <c r="X26" t="s">
-        <v>90</v>
+        <v>1974072600</v>
+      </c>
+      <c r="X26" s="1">
+        <v>44764</v>
       </c>
       <c r="Y26" s="1">
-        <v>44844</v>
-      </c>
-      <c r="Z26">
-        <v>1981004520</v>
+        <v>44764</v>
       </c>
       <c r="AA26">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AB26">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="AC26" t="s">
         <v>4</v>
       </c>
       <c r="AD26" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AE26" t="s">
         <v>11</v>
       </c>
       <c r="AF26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AG26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH26" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="AI26" t="s">
         <v>11</v>
@@ -4656,22 +4607,28 @@
       <c r="AK26" t="s">
         <v>14</v>
       </c>
+      <c r="AL26" t="s">
+        <v>11</v>
+      </c>
       <c r="AM26" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AN26" t="s">
         <v>11</v>
       </c>
+      <c r="AO26" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -4689,64 +4646,64 @@
         <v>4</v>
       </c>
       <c r="I27" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="J27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K27" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="L27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M27">
-        <v>1978330320</v>
+        <v>1978243560</v>
       </c>
       <c r="N27" s="1">
-        <v>44813</v>
+        <v>44812</v>
       </c>
       <c r="O27">
-        <v>1978899120</v>
+        <v>1978812360</v>
       </c>
       <c r="P27" s="1">
-        <v>44819</v>
+        <v>44818</v>
       </c>
       <c r="Q27">
         <v>2</v>
       </c>
       <c r="R27" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="S27" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="T27" t="s">
+        <v>44</v>
+      </c>
+      <c r="U27" t="s">
+        <v>122</v>
+      </c>
+      <c r="V27" s="1">
+        <v>44819</v>
+      </c>
+      <c r="W27">
+        <v>1978866000</v>
+      </c>
+      <c r="X27" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y27" s="1">
+        <v>44819</v>
+      </c>
+      <c r="Z27">
+        <v>1978891200</v>
+      </c>
+      <c r="AA27">
         <v>8</v>
       </c>
-      <c r="U27" t="s">
-        <v>89</v>
-      </c>
-      <c r="V27" s="1">
-        <v>44829</v>
-      </c>
-      <c r="W27">
-        <v>1979701200</v>
-      </c>
-      <c r="X27" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y27" s="1">
-        <v>44829</v>
-      </c>
-      <c r="Z27">
-        <v>1979760600</v>
-      </c>
-      <c r="AA27">
-        <v>17</v>
-      </c>
       <c r="AB27">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AC27" t="s">
         <v>4</v>
@@ -4779,24 +4736,24 @@
         <v>11</v>
       </c>
       <c r="AN27" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="F28" t="s">
         <v>4</v>
@@ -4808,64 +4765,64 @@
         <v>4</v>
       </c>
       <c r="I28" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="J28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K28" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="L28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M28">
-        <v>1972886400</v>
+        <v>1978243560</v>
       </c>
       <c r="N28" s="1">
-        <v>44750</v>
+        <v>44812</v>
       </c>
       <c r="O28">
-        <v>1973455200</v>
+        <v>1978812360</v>
       </c>
       <c r="P28" s="1">
-        <v>44756</v>
+        <v>44818</v>
       </c>
       <c r="Q28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R28" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="S28" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="T28" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="U28" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
       <c r="V28" s="1">
-        <v>44777</v>
+        <v>44831</v>
       </c>
       <c r="W28">
-        <v>1975224780</v>
+        <v>1979916300</v>
       </c>
       <c r="X28" t="s">
-        <v>63</v>
+        <v>125</v>
       </c>
       <c r="Y28" s="1">
-        <v>44792</v>
+        <v>44831</v>
       </c>
       <c r="Z28">
-        <v>1976517900</v>
+        <v>1979920800</v>
       </c>
       <c r="AA28">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="AB28">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="AC28" t="s">
         <v>4</v>
@@ -4901,21 +4858,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
@@ -4927,58 +4884,64 @@
         <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K29" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="L29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M29">
-        <v>1965456180</v>
+        <v>1978243560</v>
       </c>
       <c r="N29" s="1">
-        <v>44664</v>
+        <v>44812</v>
       </c>
       <c r="O29">
-        <v>1966024980</v>
+        <v>1978812360</v>
       </c>
       <c r="P29" s="1">
-        <v>44670</v>
+        <v>44818</v>
       </c>
       <c r="Q29">
         <v>1</v>
       </c>
       <c r="R29" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="S29" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="T29" t="s">
-        <v>20</v>
-      </c>
-      <c r="U29" s="1">
-        <v>44673</v>
+        <v>44</v>
+      </c>
+      <c r="U29" t="s">
+        <v>119</v>
       </c>
       <c r="V29" s="1">
-        <v>44673</v>
-      </c>
-      <c r="X29" s="1">
-        <v>44685</v>
+        <v>44812</v>
+      </c>
+      <c r="W29">
+        <v>1978243560</v>
+      </c>
+      <c r="X29" t="s">
+        <v>120</v>
       </c>
       <c r="Y29" s="1">
-        <v>44685</v>
+        <v>44815</v>
+      </c>
+      <c r="Z29">
+        <v>1978507020</v>
       </c>
       <c r="AA29">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AB29">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="AC29" t="s">
         <v>4</v>
@@ -4990,39 +4953,39 @@
         <v>11</v>
       </c>
       <c r="AF29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH29" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AI29" t="s">
         <v>11</v>
       </c>
       <c r="AJ29" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="AK29" t="s">
         <v>14</v>
       </c>
       <c r="AM29" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AN29" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C30" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -5052,49 +5015,49 @@
         <v>4</v>
       </c>
       <c r="M30">
-        <v>1979971200</v>
+        <v>1978935300</v>
       </c>
       <c r="N30" s="1">
-        <v>44832</v>
+        <v>44820</v>
       </c>
       <c r="O30">
-        <v>1980540000</v>
+        <v>1979504100</v>
       </c>
       <c r="P30" s="1">
-        <v>44838</v>
+        <v>44826</v>
       </c>
       <c r="Q30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R30" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="S30" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="T30" t="s">
-        <v>8</v>
-      </c>
-      <c r="U30" s="1">
-        <v>44837</v>
+        <v>79</v>
+      </c>
+      <c r="U30" t="s">
+        <v>130</v>
       </c>
       <c r="V30" s="1">
-        <v>44837</v>
-      </c>
-      <c r="X30" t="s">
-        <v>135</v>
+        <v>44851</v>
+      </c>
+      <c r="W30">
+        <v>1981612800</v>
+      </c>
+      <c r="X30" s="1">
+        <v>44858</v>
       </c>
       <c r="Y30" s="1">
-        <v>44839</v>
-      </c>
-      <c r="Z30">
-        <v>1980573300</v>
+        <v>44858</v>
       </c>
       <c r="AA30">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="AB30">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="AC30" t="s">
         <v>4</v>
@@ -5115,10 +5078,10 @@
         <v>21</v>
       </c>
       <c r="AI30" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AJ30" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="AK30" t="s">
         <v>14</v>
@@ -5127,24 +5090,24 @@
         <v>11</v>
       </c>
       <c r="AN30" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:41" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="F31" t="s">
         <v>4</v>
@@ -5168,67 +5131,70 @@
         <v>4</v>
       </c>
       <c r="M31">
-        <v>1972886580</v>
+        <v>1978935300</v>
       </c>
       <c r="N31" s="1">
-        <v>44750</v>
+        <v>44820</v>
       </c>
       <c r="O31">
-        <v>1973455380</v>
+        <v>1979504100</v>
       </c>
       <c r="P31" s="1">
-        <v>44756</v>
+        <v>44826</v>
       </c>
       <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="R31" t="s">
+        <v>42</v>
+      </c>
+      <c r="S31" t="s">
+        <v>43</v>
+      </c>
+      <c r="T31" t="s">
+        <v>44</v>
+      </c>
+      <c r="U31" t="s">
+        <v>128</v>
+      </c>
+      <c r="V31" s="1">
+        <v>44850</v>
+      </c>
+      <c r="W31">
+        <v>1981540800</v>
+      </c>
+      <c r="X31" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y31" s="1">
+        <v>44852</v>
+      </c>
+      <c r="Z31">
+        <v>1981699200</v>
+      </c>
+      <c r="AA31">
+        <v>31</v>
+      </c>
+      <c r="AB31">
+        <v>33</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF31">
         <v>2</v>
       </c>
-      <c r="R31" t="s">
-        <v>66</v>
-      </c>
-      <c r="S31" t="s">
-        <v>67</v>
-      </c>
-      <c r="T31" t="s">
-        <v>31</v>
-      </c>
-      <c r="U31" t="s">
-        <v>68</v>
-      </c>
-      <c r="V31" s="1">
-        <v>44764</v>
-      </c>
-      <c r="W31">
-        <v>1974072600</v>
-      </c>
-      <c r="X31" s="1">
-        <v>44796</v>
-      </c>
-      <c r="Y31" s="1">
-        <v>44796</v>
-      </c>
-      <c r="AA31">
-        <v>15</v>
-      </c>
-      <c r="AB31">
-        <v>47</v>
-      </c>
-      <c r="AC31" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD31" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE31" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF31">
-        <v>3</v>
-      </c>
       <c r="AG31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH31" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="AI31" t="s">
         <v>11</v>
@@ -5239,17 +5205,11 @@
       <c r="AK31" t="s">
         <v>14</v>
       </c>
-      <c r="AL31" t="s">
-        <v>11</v>
-      </c>
       <c r="AM31" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AN31" t="s">
         <v>11</v>
-      </c>
-      <c r="AO31" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:41" x14ac:dyDescent="0.2">
@@ -5257,16 +5217,16 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>131</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="F32" t="s">
         <v>4</v>
@@ -5290,105 +5250,99 @@
         <v>4</v>
       </c>
       <c r="M32">
-        <v>1972886580</v>
+        <v>1979971200</v>
       </c>
       <c r="N32" s="1">
-        <v>44750</v>
+        <v>44832</v>
       </c>
       <c r="O32">
-        <v>1973455380</v>
+        <v>1980540000</v>
       </c>
       <c r="P32" s="1">
-        <v>44756</v>
+        <v>44838</v>
       </c>
       <c r="Q32">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R32" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="S32" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="T32" t="s">
-        <v>31</v>
-      </c>
-      <c r="U32" t="s">
-        <v>68</v>
+        <v>8</v>
+      </c>
+      <c r="U32" s="1">
+        <v>44837</v>
       </c>
       <c r="V32" s="1">
-        <v>44764</v>
-      </c>
-      <c r="W32">
-        <v>1974072600</v>
-      </c>
-      <c r="X32" s="1">
-        <v>44826</v>
+        <v>44837</v>
+      </c>
+      <c r="X32" t="s">
+        <v>135</v>
       </c>
       <c r="Y32" s="1">
-        <v>44826</v>
+        <v>44839</v>
+      </c>
+      <c r="Z32">
+        <v>1980573300</v>
       </c>
       <c r="AA32">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AB32">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="AC32" t="s">
         <v>4</v>
       </c>
       <c r="AD32" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AE32" t="s">
         <v>11</v>
       </c>
       <c r="AF32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH32" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="AI32" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AJ32" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="AK32" t="s">
         <v>14</v>
       </c>
-      <c r="AL32" t="s">
-        <v>11</v>
-      </c>
       <c r="AM32" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AN32" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO32" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>136</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>137</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="F33" t="s">
         <v>4</v>
@@ -5412,108 +5366,102 @@
         <v>4</v>
       </c>
       <c r="M33">
-        <v>1972886580</v>
+        <v>1979971380</v>
       </c>
       <c r="N33" s="1">
-        <v>44750</v>
+        <v>44832</v>
       </c>
       <c r="O33">
-        <v>1973455380</v>
+        <v>1980540180</v>
       </c>
       <c r="P33" s="1">
-        <v>44756</v>
+        <v>44838</v>
       </c>
       <c r="Q33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R33" t="s">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="S33" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="T33" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="U33" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="V33" s="1">
-        <v>44764</v>
+        <v>44838</v>
       </c>
       <c r="W33">
-        <v>1974072600</v>
+        <v>1980514380</v>
       </c>
       <c r="X33" t="s">
-        <v>73</v>
+        <v>139</v>
       </c>
       <c r="Y33" s="1">
-        <v>44764</v>
+        <v>44839</v>
       </c>
       <c r="Z33">
-        <v>1974072660</v>
+        <v>1980567120</v>
       </c>
       <c r="AA33">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="AB33">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="AC33" t="s">
         <v>4</v>
       </c>
       <c r="AD33" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AE33" t="s">
         <v>11</v>
       </c>
       <c r="AF33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AG33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH33" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="AI33" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AJ33" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="AK33" t="s">
         <v>14</v>
       </c>
-      <c r="AL33" t="s">
-        <v>11</v>
-      </c>
       <c r="AM33" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AN33" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO33" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>141</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="F34" t="s">
         <v>4</v>
@@ -5537,101 +5485,112 @@
         <v>4</v>
       </c>
       <c r="M34">
-        <v>1972886580</v>
+        <v>1981180980</v>
       </c>
       <c r="N34" s="1">
-        <v>44750</v>
+        <v>44846</v>
       </c>
       <c r="O34">
-        <v>1973455380</v>
+        <v>1981749780</v>
       </c>
       <c r="P34" s="1">
-        <v>44756</v>
+        <v>44852</v>
       </c>
       <c r="Q34">
         <v>1</v>
       </c>
       <c r="R34" t="s">
-        <v>77</v>
+        <v>142</v>
       </c>
       <c r="S34" t="s">
-        <v>78</v>
+        <v>143</v>
       </c>
       <c r="T34" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="U34" t="s">
-        <v>68</v>
+        <v>144</v>
       </c>
       <c r="V34" s="1">
-        <v>44764</v>
+        <v>44847</v>
       </c>
       <c r="W34">
-        <v>1974072600</v>
-      </c>
-      <c r="X34" s="1">
-        <v>44764</v>
+        <v>1981266180</v>
+      </c>
+      <c r="X34" t="s">
+        <v>145</v>
       </c>
       <c r="Y34" s="1">
-        <v>44764</v>
+        <v>44855</v>
+      </c>
+      <c r="Z34">
+        <v>1981959300</v>
       </c>
       <c r="AA34">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="AB34">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AC34" t="s">
         <v>4</v>
       </c>
       <c r="AD34" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AE34" t="s">
         <v>11</v>
       </c>
       <c r="AF34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AG34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH34" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="AI34" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AJ34" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="AK34" t="s">
         <v>14</v>
       </c>
-      <c r="AL34" t="s">
-        <v>11</v>
-      </c>
       <c r="AM34" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AN34" t="s">
         <v>11</v>
       </c>
-      <c r="AO34" t="s">
-        <v>70</v>
-      </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
       <c r="N36" s="1"/>
       <c r="P36" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AO34" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AO34">
-      <sortCondition ref="AH1:AH34"/>
-    </sortState>
+    <filterColumn colId="34">
+      <filters>
+        <filter val="Y"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="AH1:AH34">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Grade 4">
+      <formula>NOT(ISERROR(SEARCH("Grade 4",AH1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="GRADE 1">
+      <formula>NOT(ISERROR(SEARCH("GRADE 1",AH1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="GRADE 2">
+      <formula>NOT(ISERROR(SEARCH("GRADE 2",AH1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="GRADE 3">
+      <formula>NOT(ISERROR(SEARCH("GRADE 3",AH1)))</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -5639,18 +5598,6 @@
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEF9C"/>
       </colorScale>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="GRADE 3">
-      <formula>NOT(ISERROR(SEARCH("GRADE 3",AH1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="GRADE 2">
-      <formula>NOT(ISERROR(SEARCH("GRADE 2",AH1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="GRADE 1">
-      <formula>NOT(ISERROR(SEARCH("GRADE 1",AH1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Grade 4">
-      <formula>NOT(ISERROR(SEARCH("Grade 4",AH1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5677,8 +5624,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007B36C47C1C5CBF428DE3D886D66F1FFB" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6590931cb5d23b986ab2157aebfc7a07">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="84d98a7d-1acb-47a2-b5f7-f7535c8ff9c8" xmlns:ns3="620b9a2a-88cc-4ce3-90c0-c9cc3c172a70" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd15bdabf04b9f4191b7248a0ac5945" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007B36C47C1C5CBF428DE3D886D66F1FFB" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ec57fd46265cdb6b5a27e3ee2943c41e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="84d98a7d-1acb-47a2-b5f7-f7535c8ff9c8" xmlns:ns3="620b9a2a-88cc-4ce3-90c0-c9cc3c172a70" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb1ddec0d468951bd51f82059ddd98cd" ns2:_="" ns3:_="">
     <xsd:import namespace="84d98a7d-1acb-47a2-b5f7-f7535c8ff9c8"/>
     <xsd:import namespace="620b9a2a-88cc-4ce3-90c0-c9cc3c172a70"/>
     <xsd:element name="properties">
@@ -5916,16 +5863,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BF3E8E-0308-44B8-9CC3-B2E8D9232EA7}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="620b9a2a-88cc-4ce3-90c0-c9cc3c172a70"/>
+    <ds:schemaRef ds:uri="84d98a7d-1acb-47a2-b5f7-f7535c8ff9c8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="84d98a7d-1acb-47a2-b5f7-f7535c8ff9c8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="620b9a2a-88cc-4ce3-90c0-c9cc3c172a70"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5939,5 +5886,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E77B9E5-F51D-41B1-B46A-636486CCA973}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5668D4-E404-4BCF-857F-878673F23748}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="84d98a7d-1acb-47a2-b5f7-f7535c8ff9c8"/>
+    <ds:schemaRef ds:uri="620b9a2a-88cc-4ce3-90c0-c9cc3c172a70"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>